<commit_message>
Add Thabang Github username in 2409PTDS.xlsx
</commit_message>
<xml_diff>
--- a/Github Repos 2409PTDS.xlsx
+++ b/Github Repos 2409PTDS.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>Thabang Mathebula</t>
+  </si>
+  <si>
+    <t>thabanglwazi</t>
   </si>
 </sst>
 </file>
@@ -85,7 +88,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -95,7 +98,6 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -336,7 +338,9 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>